<commit_message>
aded Brakes area missing data
</commit_message>
<xml_diff>
--- a/xml/Porsche_Nuts_and_Bolts.xlsx
+++ b/xml/Porsche_Nuts_and_Bolts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d6418f5b8b750208/Code/356_parts/xml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="637" documentId="8_{08365CD5-F318-9946-A7DC-86CF9963F12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7589545D-BCAB-F642-9214-D34AFA9576AC}"/>
+  <xr:revisionPtr revIDLastSave="639" documentId="8_{08365CD5-F318-9946-A7DC-86CF9963F12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25D43A20-4173-C74C-927F-35927B700136}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="group3-4" sheetId="6" r:id="rId1"/>
@@ -1324,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8419CACA-44BF-1546-811D-F9987A0E7488}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -2943,8 +2943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C62653-3715-0C4A-BD42-BE332B90BAE6}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
change popup to table row
</commit_message>
<xml_diff>
--- a/xml/Porsche_Nuts_and_Bolts.xlsx
+++ b/xml/Porsche_Nuts_and_Bolts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d6418f5b8b750208/Code/356_parts/xml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="639" documentId="8_{08365CD5-F318-9946-A7DC-86CF9963F12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25D43A20-4173-C74C-927F-35927B700136}"/>
+  <xr:revisionPtr revIDLastSave="779" documentId="8_{08365CD5-F318-9946-A7DC-86CF9963F12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98A19B1E-FE7D-EC42-86F5-B0B43A0B5D15}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="14700" windowHeight="16680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="group3-4" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="246">
   <si>
     <t>Size</t>
   </si>
@@ -629,6 +629,138 @@
   </si>
   <si>
     <t>47B</t>
+  </si>
+  <si>
+    <t>19B</t>
+  </si>
+  <si>
+    <t>23B</t>
+  </si>
+  <si>
+    <t>24B</t>
+  </si>
+  <si>
+    <t>21B</t>
+  </si>
+  <si>
+    <t>22B</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Fastening screw for bearing cover</t>
+  </si>
+  <si>
+    <t>P 901.401</t>
+  </si>
+  <si>
+    <t>heaxagon bolt</t>
+  </si>
+  <si>
+    <t>M12x1.5x22</t>
+  </si>
+  <si>
+    <t>no part number provided</t>
+  </si>
+  <si>
+    <t>washer for bearing housing</t>
+  </si>
+  <si>
+    <t>356.34.153</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>hexagin nut</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>check whether this is a wave washer</t>
+  </si>
+  <si>
+    <t>900.028.014.01</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>900.082.006.01</t>
+  </si>
+  <si>
+    <t>M12x1.5x30</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>hexagin nut self locking</t>
+  </si>
+  <si>
+    <t>900.084.013.02</t>
+  </si>
+  <si>
+    <t>DIN 985-6S</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>n644.333.564.10</t>
+  </si>
+  <si>
+    <t>no size or finish specified</t>
+  </si>
+  <si>
+    <t>28B</t>
+  </si>
+  <si>
+    <t>29B</t>
+  </si>
+  <si>
+    <t>44B</t>
+  </si>
+  <si>
+    <t>43B</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>bolt for ribber buffer</t>
+  </si>
+  <si>
+    <t>695.333.513.00</t>
   </si>
 </sst>
 </file>
@@ -731,7 +863,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -751,6 +883,10 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,8 +1117,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L7" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:L7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L18" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:L18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L13">
+    <sortCondition ref="E1:E13"/>
+  </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="diagram_name" dataDxfId="13"/>
     <tableColumn id="12" xr3:uid="{26B54F8E-BF5D-8F46-84D4-AD3810497338}" name="ref" dataDxfId="12"/>
@@ -995,7 +1134,7 @@
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DIN" dataDxfId="5"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Size" dataDxfId="4"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Finish" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{E2BFE521-0ABD-424B-9159-1CAF84470C53}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{E2BFE521-0ABD-424B-9159-1CAF84470C53}" name="Notes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2638,10 +2777,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2702,32 +2841,32 @@
       <c r="A2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>3</v>
+      <c r="B2" s="3">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="3">
-        <v>8</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>12</v>
@@ -2740,35 +2879,35 @@
       <c r="A3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>3</v>
+      <c r="B3" s="3">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E3" s="1">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="H3" s="1">
-        <v>8</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>175</v>
@@ -2779,7 +2918,7 @@
         <v>45</v>
       </c>
       <c r="B4" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>44</v>
@@ -2788,22 +2927,22 @@
         <v>43</v>
       </c>
       <c r="E4" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="H4" s="1">
         <v>2</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>25</v>
+        <v>32</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>12</v>
@@ -2817,7 +2956,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>3</v>
@@ -2826,25 +2965,25 @@
         <v>42</v>
       </c>
       <c r="E5" s="1">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="1">
-        <v>2</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="H5" s="3">
+        <v>8</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>175</v>
@@ -2854,35 +2993,35 @@
       <c r="A6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="3">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>44</v>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="H6" s="1">
-        <v>2</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>30</v>
+        <v>8</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>175</v>
@@ -2892,43 +3031,461 @@
       <c r="A7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="3">
-        <v>16</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>44</v>
+      <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H7" s="1">
         <v>2</v>
       </c>
       <c r="I7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="K16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="6" t="s">
-        <v>175</v>
+      <c r="L16" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:B30">
-    <sortCondition ref="B8:B30"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:B26">
+    <sortCondition ref="B8:B26"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2943,8 +3500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C62653-3715-0C4A-BD42-BE332B90BAE6}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>